<commit_message>
Pilot draft ready - to 1st share
</commit_message>
<xml_diff>
--- a/legend_data.xlsx
+++ b/legend_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/shaider7_worldbank_org/Documents/RShinyProjects/CCDR_Dashboard/CCDR-World-Bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7F85CA17-6D6B-4DE8-98A7-1BD49A098296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C4A0CB3-79F2-4DB9-9442-7393A2FCF11B}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{7F85CA17-6D6B-4DE8-98A7-1BD49A098296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77B656A3-7D8A-43BF-AAA8-772926F2A15B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,30 +226,9 @@
     <t>Expected mortality from river floods (population count)</t>
   </si>
   <si>
-    <t>Expected damage on builtup from river floods (hectars)</t>
-  </si>
-  <si>
-    <t>Expected damage on agricultural land from river floods (hectars)</t>
-  </si>
-  <si>
-    <t>Frequency of agricultural stress affecting at least 30% of arable land during Season 1 (percentage of historical period 1984-2022)</t>
-  </si>
-  <si>
-    <t>Frequency of agricultural stress affecting at least 30% of arable land during Season 2 (percentage of historical period 1984-2022)</t>
-  </si>
-  <si>
-    <t>Expected impact from heat stress (population count)</t>
-  </si>
-  <si>
-    <t>Expected increse of mortality from air pollution (population count)</t>
-  </si>
-  <si>
     <t>Tehsil Population</t>
   </si>
   <si>
-    <t>District population</t>
-  </si>
-  <si>
     <t>Expected mortality from coastal floods (population count)</t>
   </si>
   <si>
@@ -265,30 +244,12 @@
     <t>Expected mortality from river floods (% of ADM population)</t>
   </si>
   <si>
-    <t>Expected damage on builtup from river floods (% of ADM builtup)</t>
-  </si>
-  <si>
-    <t>Expected damage on agricultural land from river floods (% of ADM builtup)</t>
-  </si>
-  <si>
-    <t>Expected impact from heat stress (% of ADM population)</t>
-  </si>
-  <si>
-    <t>Expected increse of mortality from air pollution (% of ADM population)</t>
-  </si>
-  <si>
     <t>Built-up area extent (Ha)</t>
   </si>
   <si>
     <t>Agricultural land extent (Ha)</t>
   </si>
   <si>
-    <t>Expected damage on builtup from coastal floods (% of ADM builtup)</t>
-  </si>
-  <si>
-    <t>Expected damage on builtup from coastal floods (hectars)</t>
-  </si>
-  <si>
     <t>(000's)</t>
   </si>
   <si>
@@ -301,16 +262,55 @@
     <t>(Per Sq-Km)</t>
   </si>
   <si>
-    <t>Population exposed to medium or high hazard - Land Slides (population count)</t>
-  </si>
-  <si>
-    <t>Population exposed to medium or high hazard - Land Slides (% of ADM population)</t>
-  </si>
-  <si>
-    <t>Builtup exposed to medium or high hazard -Land Slides (Builtup count)</t>
-  </si>
-  <si>
-    <t>Builtup exposed to medium or high hazard - Land Slides (% of ADM Builtup)</t>
+    <t>Expected damage to built-up assets from river floods (hectares)</t>
+  </si>
+  <si>
+    <t>Expected damage to built-up assets from river floods (% of ADM built-up area)</t>
+  </si>
+  <si>
+    <t>Expected exposure of agricultural land to river floods (hectares)</t>
+  </si>
+  <si>
+    <t>Expected exposure of agricultural land to river floods (% of ADM agricultural land)</t>
+  </si>
+  <si>
+    <t>Expected damage to built-up assets from coastal floods (hectares)</t>
+  </si>
+  <si>
+    <t>Expected damage to built-up assets from coastal floods (% of ADM built-up area)</t>
+  </si>
+  <si>
+    <t>Population exposed to medium or high landslide hazard (population count)</t>
+  </si>
+  <si>
+    <t>Population exposed to medium or high landslide hazard (% of ADM population)</t>
+  </si>
+  <si>
+    <t>Built-up assets exposed to medium or high landslide hazard (Hectares)</t>
+  </si>
+  <si>
+    <t>Built-up assets exposed to medium or high landslide hazard (% of ADM built-up area)</t>
+  </si>
+  <si>
+    <t>Frequency of agricultural drought stress affecting at least 30% of arable land during Season 1/Kharif (percentage of historical period 1984-2022)</t>
+  </si>
+  <si>
+    <t>Frequency of agricultural drought stress affecting at least 30% of arable land during Season 2/Rabi (percentage of historical period 1984-2022)</t>
+  </si>
+  <si>
+    <t>Expected exposure to heat stress (population count)</t>
+  </si>
+  <si>
+    <t>Expected exposure to heat stress (% of ADM population)</t>
+  </si>
+  <si>
+    <t>Expected increase of mortality from air pollution (population count)</t>
+  </si>
+  <si>
+    <t>Expected increase of mortality from air pollution (% of ADM population)</t>
+  </si>
+  <si>
+    <t>District Population</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,13 +692,13 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -709,13 +709,13 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -726,13 +726,13 @@
         <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
         <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -757,13 +757,13 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
         <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -774,13 +774,13 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
         <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -791,7 +791,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
         <v>65</v>
@@ -808,13 +808,13 @@
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
         <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -825,13 +825,13 @@
         <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
         <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -845,7 +845,7 @@
         <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -856,13 +856,13 @@
         <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
         <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -876,7 +876,7 @@
         <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -887,13 +887,13 @@
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
         <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -907,7 +907,7 @@
         <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -918,13 +918,13 @@
         <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
         <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -938,7 +938,7 @@
         <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -949,13 +949,13 @@
         <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
         <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -969,7 +969,7 @@
         <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -983,7 +983,7 @@
         <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -997,7 +997,7 @@
         <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1008,13 +1008,13 @@
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
         <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1028,7 +1028,7 @@
         <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1039,13 +1039,13 @@
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
         <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1056,13 +1056,13 @@
         <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
         <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1073,13 +1073,13 @@
         <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1090,13 +1090,13 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
         <v>65</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
         <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
         <v>65</v>
@@ -1124,7 +1124,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
         <v>65</v>
@@ -1141,7 +1141,7 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
         <v>65</v>
@@ -1158,7 +1158,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
         <v>65</v>
@@ -1175,7 +1175,7 @@
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
         <v>65</v>
@@ -1192,7 +1192,7 @@
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
         <v>65</v>
@@ -1209,7 +1209,7 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
         <v>65</v>
@@ -1226,7 +1226,7 @@
         <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
         <v>65</v>
@@ -1243,7 +1243,7 @@
         <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
         <v>65</v>
@@ -1260,7 +1260,7 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
         <v>65</v>
@@ -1277,7 +1277,7 @@
         <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
         <v>65</v>
@@ -1294,7 +1294,7 @@
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
         <v>65</v>
@@ -1311,7 +1311,7 @@
         <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
         <v>65</v>
@@ -1328,7 +1328,7 @@
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
         <v>65</v>
@@ -1345,7 +1345,7 @@
         <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
         <v>65</v>
@@ -1362,7 +1362,7 @@
         <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
         <v>65</v>
@@ -1379,7 +1379,7 @@
         <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
         <v>65</v>
@@ -1396,7 +1396,7 @@
         <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
         <v>65</v>
@@ -1413,7 +1413,7 @@
         <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
         <v>65</v>
@@ -1430,7 +1430,7 @@
         <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D47" t="s">
         <v>65</v>
@@ -1489,7 +1489,7 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D51" t="s">
         <v>65</v>
@@ -1506,7 +1506,7 @@
         <v>61</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D52" t="s">
         <v>65</v>
@@ -1551,7 +1551,7 @@
         <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D55" t="s">
         <v>65</v>
@@ -1568,7 +1568,7 @@
         <v>61</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D56" t="s">
         <v>65</v>
@@ -1585,7 +1585,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
         <v>65</v>
@@ -1602,7 +1602,7 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D58" t="s">
         <v>65</v>
@@ -1619,7 +1619,7 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D59" t="s">
         <v>65</v>
@@ -1636,7 +1636,7 @@
         <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D60" t="s">
         <v>65</v>
@@ -1707,6 +1707,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Relative Wealth index prep and added across the dashboard
</commit_message>
<xml_diff>
--- a/legend_data.xlsx
+++ b/legend_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/shaider7_worldbank_org/Documents/RShinyProjects/CCDR_Dashboard/CCDR-World-Bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="13_ncr:1_{7F85CA17-6D6B-4DE8-98A7-1BD49A098296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0341C707-7C12-4551-B62C-C8CBBC2A00EA}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="13_ncr:1_{7F85CA17-6D6B-4DE8-98A7-1BD49A098296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38E3967E-9406-40B3-88FE-EE831BA9C708}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="165">
   <si>
     <t>indicator</t>
   </si>
@@ -500,6 +500,21 @@
   </si>
   <si>
     <t>Share of population Living in Area with Low Road Density (OpenStreetMap 2022)</t>
+  </si>
+  <si>
+    <t>Mean Relative Wealth Index</t>
+  </si>
+  <si>
+    <t>Majority Relative Wealth Index</t>
+  </si>
+  <si>
+    <t>RWI_rwi_mean</t>
+  </si>
+  <si>
+    <t>RWI_rwi_majority</t>
+  </si>
+  <si>
+    <t>Pakistan Poverty Team - World Bank</t>
   </si>
 </sst>
 </file>
@@ -876,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53:E55"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2047,6 +2062,40 @@
         <v>151</v>
       </c>
     </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>162</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" t="s">
+        <v>164</v>
+      </c>
+      <c r="E61" t="s">
+        <v>160</v>
+      </c>
+      <c r="F61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>163</v>
+      </c>
+      <c r="B62" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E62" t="s">
+        <v>161</v>
+      </c>
+      <c r="F62" t="s">
+        <v>161</v>
+      </c>
+    </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="1"/>
     </row>

</xml_diff>